<commit_message>
Updated wireframe and blog
</commit_message>
<xml_diff>
--- a/documentation/ExcelFiles/Sprint2backlog.xlsx
+++ b/documentation/ExcelFiles/Sprint2backlog.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26717"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16300b0c7e6b1157/Bureau/McGill1/CapstoneProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="8_{ED1A4A1A-18E7-45F0-BC40-36A4F0AA9B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3288BBA3-949D-46BC-B82D-7A9135513195}"/>
+  <xr:revisionPtr revIDLastSave="171" documentId="8_{ED1A4A1A-18E7-45F0-BC40-36A4F0AA9B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5D228FF-C9C8-45FC-A979-F82CA98EACB4}"/>
   <bookViews>
     <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{11D63FB2-F6E9-4BF0-8080-3A9F2DF79420}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+  <si>
+    <t>Sprint 2 Backlog</t>
+  </si>
   <si>
     <t>Story ID</t>
   </si>
@@ -59,83 +62,98 @@
     <t>Comments</t>
   </si>
   <si>
+    <t>BK-2</t>
+  </si>
+  <si>
+    <t>BK-2.1</t>
+  </si>
+  <si>
+    <t>Administrator sign up page</t>
+  </si>
+  <si>
+    <t>Administrator form page and input fields validation</t>
+  </si>
+  <si>
+    <t>5 hrs</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>BK-2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrator call API </t>
+  </si>
+  <si>
+    <t>Submit administrator form data to call API and send data to back end</t>
+  </si>
+  <si>
     <t>1.5 hrs</t>
   </si>
   <si>
-    <t>5 hrs</t>
+    <t>BK-2.3</t>
+  </si>
+  <si>
+    <t>Restore registration form data to db</t>
+  </si>
+  <si>
+    <t>provide register api for administrator, receive the form data and insert into database</t>
+  </si>
+  <si>
+    <t>2 hrs</t>
+  </si>
+  <si>
+    <t>BK-2.4</t>
+  </si>
+  <si>
+    <t>Wireframes</t>
+  </si>
+  <si>
+    <t>Create and modify wireframes</t>
   </si>
   <si>
     <t>4 hrs</t>
   </si>
   <si>
-    <t>BK-2</t>
-  </si>
-  <si>
-    <t>2 hrs</t>
-  </si>
-  <si>
-    <t>Sprint 2 Backlog</t>
-  </si>
-  <si>
-    <t>Administrator sign up page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Administrator call API </t>
-  </si>
-  <si>
-    <t>Restore registration form data to db</t>
-  </si>
-  <si>
-    <t>Administrator form page and input fields validation</t>
-  </si>
-  <si>
-    <t>Submit administrator form data to call API and send data to back end</t>
-  </si>
-  <si>
-    <t>provide register api for administrator, receive the form data and insert into database</t>
-  </si>
-  <si>
-    <t>in progress</t>
-  </si>
-  <si>
-    <t>BK-2.1</t>
-  </si>
-  <si>
-    <t>BK-2.2</t>
-  </si>
-  <si>
-    <t>BK-2.3</t>
-  </si>
-  <si>
-    <t>BK-2.4</t>
-  </si>
-  <si>
-    <t>Create and modify wireframes</t>
-  </si>
-  <si>
-    <t>Wireframes</t>
+    <t>BK-2.5</t>
   </si>
   <si>
     <t>Diagrams</t>
   </si>
   <si>
+    <t xml:space="preserve">Provide detailed diagrams (Database,use-case) </t>
+  </si>
+  <si>
     <t>3 hrs</t>
   </si>
   <si>
-    <t>BK-2.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Provide detailed diagrams (Database,use-case) </t>
-  </si>
-  <si>
     <t>BK-2.6</t>
+  </si>
+  <si>
+    <t>Contactus page</t>
+  </si>
+  <si>
+    <t>Setup page and add styling</t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t>BK-2.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contactus page </t>
+  </si>
+  <si>
+    <t>Added API key for Sendpulse to allow visiters to send email via the contact us page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +168,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -349,79 +373,76 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -737,206 +758,314 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B7243F0-352B-4836-B41F-A56B52E75942}">
-  <dimension ref="A3:H13"/>
+  <dimension ref="A3:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:10" ht="15">
+      <c r="A3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="15">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" ht="15">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" ht="45.75">
+      <c r="A6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="8"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="13" t="s">
+      <c r="G6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" ht="45.75">
+      <c r="A7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="17"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" ht="72.599999999999994" customHeight="1">
+      <c r="A8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="E8" s="17"/>
+      <c r="F8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="14" t="s">
+      <c r="H8" s="19"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" ht="30.75">
+      <c r="A9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="21"/>
-    </row>
-    <row r="7" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="17"/>
-    </row>
-    <row r="8" spans="1:8" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="13" t="s">
+      <c r="B9" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="20"/>
-    </row>
-    <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="13" t="s">
+      <c r="C9" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="D9" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="17"/>
+      <c r="F9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="20"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="22" t="s">
+      <c r="G9" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="19"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" ht="15">
+      <c r="A10" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>29</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H10" s="17"/>
-    </row>
-    <row r="11" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="23"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="24"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" ht="14.45" customHeight="1">
+      <c r="A11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
-    </row>
-    <row r="12" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="23"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="24"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" ht="14.45" customHeight="1">
+      <c r="A12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="13" t="s">
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" ht="30.75">
+      <c r="A13" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="C13" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" ht="36.75" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" ht="15">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" ht="15">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" ht="15">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" customHeight="1">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="D4:E5"/>
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="G10:H12"/>
     <mergeCell ref="B4:B5"/>
@@ -952,14 +1081,6 @@
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="D4:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>